<commit_message>
Put in resting muscle length for extensor 10 mm
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B49084-AFB4-4EAE-AF5E-4879EDDE7775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B57C96-F8AC-4DBA-8F04-B963D8D30BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27240" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-25365" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="FlxTest1" sheetId="2" r:id="rId1"/>
-    <sheet name="ExtTest1" sheetId="1" r:id="rId2"/>
+    <sheet name="Test1" sheetId="2" r:id="rId1"/>
+    <sheet name="FlxTest1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>Test #</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>expected max contract</t>
-  </si>
-  <si>
-    <t>Flexor Test 10mm</t>
   </si>
   <si>
     <t>Extensor Test 10mm</t>
@@ -594,7 +591,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -618,7 +617,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>416</v>
+        <v>520</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -627,7 +626,7 @@
       </c>
       <c r="C3">
         <f>C2-C2*0.17</f>
-        <v>345.28</v>
+        <v>431.6</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -869,63 +868,63 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <f>C6*COS(RADIANS(C9-2.83))*C12/1000</f>
+        <f t="shared" ref="C15:Q15" si="0">C6*COS(RADIANS(C9-2.83))*C12/1000</f>
         <v>8.0576321358013914</v>
       </c>
       <c r="D15">
-        <f>D6*COS(RADIANS(D9-2.83))*D12/1000</f>
+        <f t="shared" si="0"/>
         <v>7.9233096388882238</v>
       </c>
       <c r="E15">
-        <f>E6*COS(RADIANS(E9-2.83))*E12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15">
-        <f>F6*COS(RADIANS(F9-2.83))*F12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>G6*COS(RADIANS(G9-2.83))*G12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15">
-        <f>H6*COS(RADIANS(H9-2.83))*H12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15">
-        <f>I6*COS(RADIANS(I9-2.83))*I12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J15">
-        <f>J6*COS(RADIANS(J9-2.83))*J12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K15">
-        <f>K6*COS(RADIANS(K9-2.83))*K12/1000</f>
+        <f t="shared" si="0"/>
         <v>0.68113434076134938</v>
       </c>
       <c r="L15">
-        <f>L6*COS(RADIANS(L9-2.83))*L12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f>M6*COS(RADIANS(M9-2.83))*M12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N15">
-        <f>N6*COS(RADIANS(N9-2.83))*N12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O15">
-        <f>O6*COS(RADIANS(O9-2.83))*O12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P15">
-        <f>P6*COS(RADIANS(P9-2.83))*P12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f>Q6*COS(RADIANS(Q9-2.83))*Q12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -939,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,7 +956,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -965,7 +964,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -974,7 +973,7 @@
       </c>
       <c r="C3">
         <f>C2-C2*0.17</f>
-        <v>345.28</v>
+        <v>344.45</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1343,63 +1342,63 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <f>C6*COS(RADIANS(C9-2.83))*C12/1000</f>
+        <f t="shared" ref="C15:Q15" si="0">C6*COS(RADIANS(C9-2.83))*C12/1000</f>
         <v>8.0576321358013914</v>
       </c>
       <c r="D15">
-        <f>D6*COS(RADIANS(D9-2.83))*D12/1000</f>
+        <f t="shared" si="0"/>
         <v>7.9233096388882238</v>
       </c>
       <c r="E15">
-        <f>E6*COS(RADIANS(E9-2.83))*E12/1000</f>
+        <f t="shared" si="0"/>
         <v>7.304428468107508</v>
       </c>
       <c r="F15">
-        <f>F6*COS(RADIANS(F9-2.83))*F12/1000</f>
+        <f t="shared" si="0"/>
         <v>5.4337057127252448</v>
       </c>
       <c r="G15">
-        <f>G6*COS(RADIANS(G9-2.83))*G12/1000</f>
+        <f t="shared" si="0"/>
         <v>3.8555189452627423</v>
       </c>
       <c r="H15">
-        <f>H6*COS(RADIANS(H9-2.83))*H12/1000</f>
+        <f t="shared" si="0"/>
         <v>2.6008191373026679</v>
       </c>
       <c r="I15">
-        <f>I6*COS(RADIANS(I9-2.83))*I12/1000</f>
+        <f t="shared" si="0"/>
         <v>2.3118280235883155</v>
       </c>
       <c r="J15">
-        <f>J6*COS(RADIANS(J9-2.83))*J12/1000</f>
+        <f t="shared" si="0"/>
         <v>1.3383835969396616</v>
       </c>
       <c r="K15">
-        <f>K6*COS(RADIANS(K9-2.83))*K12/1000</f>
+        <f t="shared" si="0"/>
         <v>0.8940302221017159</v>
       </c>
       <c r="L15">
-        <f>L6*COS(RADIANS(L9-2.83))*L12/1000</f>
+        <f t="shared" si="0"/>
         <v>0.35534206680410968</v>
       </c>
       <c r="M15">
-        <f>M6*COS(RADIANS(M9-2.83))*M12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N15">
-        <f>N6*COS(RADIANS(N9-2.83))*N12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O15">
-        <f>O6*COS(RADIANS(O9-2.83))*O12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P15">
-        <f>P6*COS(RADIANS(P9-2.83))*P12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f>Q6*COS(RADIANS(Q9-2.83))*Q12/1000</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Did 2 10mm extensor tests
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B57C96-F8AC-4DBA-8F04-B963D8D30BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2152F0C9-6483-4D4D-8905-3962A6C3AE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25365" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-25020" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test1" sheetId="2" r:id="rId1"/>
-    <sheet name="FlxTest1" sheetId="1" r:id="rId2"/>
+    <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
+    <sheet name="FlxTest10mm" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -104,12 +104,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -256,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -275,6 +281,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,7 +602,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,13 +694,10 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>23.454999999999998</v>
+        <v>5.8230000000000004</v>
       </c>
       <c r="D6">
-        <v>23.064</v>
-      </c>
-      <c r="K6">
-        <v>2.4356</v>
+        <v>7.3517999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -698,13 +705,10 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="D7">
-        <v>11</v>
-      </c>
-      <c r="K7">
-        <v>61.5</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -715,9 +719,12 @@
         <v>12</v>
       </c>
       <c r="C8" s="2">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4"/>
+        <f>90-54.6</f>
+        <v>35.4</v>
+      </c>
+      <c r="D8" s="4">
+        <v>33.5</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -738,10 +745,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="16">
-        <v>23</v>
+        <v>33.5</v>
       </c>
       <c r="D9" s="16">
-        <v>23</v>
+        <v>35.5</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -749,9 +756,7 @@
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
-      <c r="K9" s="16">
-        <v>43</v>
-      </c>
+      <c r="K9" s="16"/>
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
@@ -765,9 +770,11 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>397</v>
-      </c>
-      <c r="D10" s="16"/>
+        <v>503</v>
+      </c>
+      <c r="D10" s="16">
+        <v>497</v>
+      </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -790,54 +797,54 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="D12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="E12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="F12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="G12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="H12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="I12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="J12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="K12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="L12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="M12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="N12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="O12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="P12" s="16">
-        <v>365.98</v>
-      </c>
-      <c r="Q12" s="16">
+      <c r="C12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="D12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="E12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="F12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="G12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="H12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="I12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="J12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="K12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="L12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="M12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="N12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="O12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="P12" s="20">
+        <v>365.98</v>
+      </c>
+      <c r="Q12" s="20">
         <v>365.98</v>
       </c>
     </row>
@@ -847,9 +854,11 @@
         <v>11</v>
       </c>
       <c r="C13" s="16">
-        <v>38</v>
-      </c>
-      <c r="D13" s="16"/>
+        <v>40</v>
+      </c>
+      <c r="D13" s="16">
+        <v>40</v>
+      </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -869,11 +878,11 @@
       </c>
       <c r="C15">
         <f t="shared" ref="C15:Q15" si="0">C6*COS(RADIANS(C9-2.83))*C12/1000</f>
-        <v>8.0576321358013914</v>
+        <v>1.8330019342714572</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>7.9233096388882238</v>
+        <v>2.2649395901487379</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
@@ -901,7 +910,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>0.68113434076134938</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Redid measurements for 2 extensor tests
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2152F0C9-6483-4D4D-8905-3962A6C3AE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8098860C-59DB-4791-B1B3-618ED541FDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25020" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-25365" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Test #</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Extensor Test 10mm</t>
+  </si>
+  <si>
+    <t>tendon</t>
   </si>
 </sst>
 </file>
@@ -602,7 +605,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,6 +642,14 @@
         <v>431.6</v>
       </c>
     </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+    </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>0</v>
@@ -694,10 +705,10 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>5.8230000000000004</v>
+        <v>16.268999999999998</v>
       </c>
       <c r="D6">
-        <v>7.3517999999999999</v>
+        <v>11.218999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -705,10 +716,10 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D7">
-        <v>114</v>
+        <v>108.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -719,11 +730,10 @@
         <v>12</v>
       </c>
       <c r="C8" s="2">
-        <f>90-54.6</f>
-        <v>35.4</v>
+        <v>33.6</v>
       </c>
       <c r="D8" s="4">
-        <v>33.5</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -745,10 +755,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="16">
-        <v>33.5</v>
+        <v>30.5</v>
       </c>
       <c r="D9" s="16">
-        <v>35.5</v>
+        <v>30</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -770,10 +780,10 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>503</v>
+        <v>518</v>
       </c>
       <c r="D10" s="16">
-        <v>497</v>
+        <v>520</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -854,10 +864,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="16">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="16">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -878,11 +888,11 @@
       </c>
       <c r="C15">
         <f t="shared" ref="C15:Q15" si="0">C6*COS(RADIANS(C9-2.83))*C12/1000</f>
-        <v>1.8330019342714572</v>
+        <v>5.2731959840514264</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>2.2649395901487379</v>
+        <v>3.6528632273951325</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Finished Extensor 10 mm data collection
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8098860C-59DB-4791-B1B3-618ED541FDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8019B41-0615-49DD-A61C-9C36395D0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25365" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
@@ -605,7 +605,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,6 +710,27 @@
       <c r="D6">
         <v>11.218999999999999</v>
       </c>
+      <c r="E6">
+        <v>10.593</v>
+      </c>
+      <c r="F6">
+        <v>11.395</v>
+      </c>
+      <c r="G6">
+        <v>10.654999999999999</v>
+      </c>
+      <c r="H6">
+        <v>7.7816000000000001</v>
+      </c>
+      <c r="I6">
+        <v>3.9580000000000002</v>
+      </c>
+      <c r="J6">
+        <v>1.909</v>
+      </c>
+      <c r="K6">
+        <v>1.22</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -721,6 +742,27 @@
       <c r="D7">
         <v>108.5</v>
       </c>
+      <c r="E7">
+        <v>93</v>
+      </c>
+      <c r="F7">
+        <v>70</v>
+      </c>
+      <c r="G7">
+        <v>53.5</v>
+      </c>
+      <c r="H7">
+        <v>49</v>
+      </c>
+      <c r="I7">
+        <v>21</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -735,13 +777,27 @@
       <c r="D8" s="4">
         <v>36.700000000000003</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="E8" s="4">
+        <v>36.1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>39</v>
+      </c>
+      <c r="G8" s="4">
+        <v>34</v>
+      </c>
+      <c r="H8" s="4">
+        <v>38.5</v>
+      </c>
+      <c r="I8" s="4">
+        <v>36.4</v>
+      </c>
+      <c r="J8" s="4">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="K8" s="4">
+        <v>34.6</v>
+      </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -760,13 +816,27 @@
       <c r="D9" s="16">
         <v>30</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="E9" s="16">
+        <v>34</v>
+      </c>
+      <c r="F9" s="16">
+        <v>42.5</v>
+      </c>
+      <c r="G9" s="16">
+        <v>40</v>
+      </c>
+      <c r="H9" s="16">
+        <v>41.5</v>
+      </c>
+      <c r="I9" s="16">
+        <v>38</v>
+      </c>
+      <c r="J9" s="16">
+        <v>38</v>
+      </c>
+      <c r="K9" s="16">
+        <v>35</v>
+      </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
@@ -785,13 +855,27 @@
       <c r="D10" s="16">
         <v>520</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="1"/>
+      <c r="E10" s="16">
+        <v>510</v>
+      </c>
+      <c r="F10" s="16">
+        <v>495</v>
+      </c>
+      <c r="G10" s="16">
+        <v>485</v>
+      </c>
+      <c r="H10" s="16">
+        <v>475</v>
+      </c>
+      <c r="I10" s="16">
+        <v>460</v>
+      </c>
+      <c r="J10" s="16">
+        <v>450</v>
+      </c>
+      <c r="K10" s="16">
+        <v>450</v>
+      </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -869,12 +953,27 @@
       <c r="D13" s="16">
         <v>35</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+      <c r="E13" s="16">
+        <v>40</v>
+      </c>
+      <c r="F13" s="16">
+        <v>40</v>
+      </c>
+      <c r="G13" s="16">
+        <v>45</v>
+      </c>
+      <c r="H13" s="16">
+        <v>45</v>
+      </c>
+      <c r="I13" s="16">
+        <v>40</v>
+      </c>
+      <c r="J13" s="16">
+        <v>40</v>
+      </c>
+      <c r="K13" s="16">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
@@ -896,31 +995,31 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.3171496121623392</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.2100537207082049</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.107315910615343</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.2235275698755532</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1841113322514456</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.57111382851642489</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.37794605186950148</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Update results with actual moment arm for extensor test
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8019B41-0615-49DD-A61C-9C36395D0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0350EDFF-AD06-4B9B-9046-DE678802D693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25365" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-25020" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
@@ -107,18 +107,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -265,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -284,10 +278,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,7 +597,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,55 +883,55 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="D12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="E12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="F12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="G12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="H12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="I12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="J12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="K12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="L12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="M12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="N12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="O12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="P12" s="20">
-        <v>365.98</v>
-      </c>
-      <c r="Q12" s="20">
-        <v>365.98</v>
+      <c r="C12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="D12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="E12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="F12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="G12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="H12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="I12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="J12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="K12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="L12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="M12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="N12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="O12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="P12" s="16">
+        <v>366.05</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>366.05</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -986,63 +978,63 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:Q15" si="0">C6*COS(RADIANS(C9-2.83))*C12/1000</f>
-        <v>5.2731959840514264</v>
+        <f>C6*COS(RADIANS(C9-3.05))*C12/1000</f>
+        <v>5.284784415964447</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>3.6528632273951325</v>
+        <f t="shared" ref="D15:K15" si="0">D6*COS(RADIANS(D9-3.05))*D12/1000</f>
+        <v>3.6607354242219894</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>3.3171496121623392</v>
+        <v>3.3254657241807237</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>3.2100537207082049</v>
+        <v>3.2208680746256029</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>3.107315910615343</v>
+        <v>3.1169354947951735</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>2.2235275698755532</v>
+        <v>2.2307704310131626</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>1.1841113322514456</v>
+        <v>1.1875334409308596</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0.57111382851642489</v>
+        <v>0.57276436046917911</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>0.37794605186950148</v>
+        <v>0.37892854031665485</v>
       </c>
       <c r="L15">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C15:Q15" si="1">L6*COS(RADIANS(L9-2.83))*L12/1000</f>
         <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1057,7 +1049,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,49 +1360,49 @@
         <v>10</v>
       </c>
       <c r="C12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="D12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="E12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="F12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="G12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="H12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="I12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="J12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="K12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="L12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="M12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="N12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="O12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="P12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
       <c r="Q12" s="16">
-        <v>365.98</v>
+        <v>366.43</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1461,43 +1453,43 @@
       </c>
       <c r="C15">
         <f t="shared" ref="C15:Q15" si="0">C6*COS(RADIANS(C9-2.83))*C12/1000</f>
-        <v>8.0576321358013914</v>
+        <v>8.0675396019501164</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>7.9233096388882238</v>
+        <v>7.9330519454008748</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>7.304428468107508</v>
+        <v>7.3134098135653147</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>5.4337057127252448</v>
+        <v>5.4403868635278192</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>3.8555189452627423</v>
+        <v>3.8602595964605353</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>2.6008191373026679</v>
+        <v>2.6040170404989795</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>2.3118280235883155</v>
+        <v>2.3146705904242482</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>1.3383835969396616</v>
+        <v>1.3400292404683321</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>0.8940302221017159</v>
+        <v>0.89512949965771826</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>0.35534206680410968</v>
+        <v>0.35577898666328733</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Organized test data, change muscle routing Location in matlab
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0350EDFF-AD06-4B9B-9046-DE678802D693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B1DF45-9852-470E-BDCD-BE9C93BF7160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25020" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-24315" yWindow="3930" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>Test #</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>tendon</t>
+  </si>
+  <si>
+    <t>Flexsor Test 10mm</t>
   </si>
 </sst>
 </file>
@@ -596,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1014,7 +1017,7 @@
         <v>0.37892854031665485</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="C15:Q15" si="1">L6*COS(RADIANS(L9-2.83))*L12/1000</f>
+        <f t="shared" ref="L15:Q15" si="1">L6*COS(RADIANS(L9-2.83))*L12/1000</f>
         <v>0</v>
       </c>
       <c r="M15">
@@ -1048,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1069,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working on plotting data
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E3E6E0-4503-4E41-84BC-68DEF138E67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA71BA0A-9BA8-4B23-BA76-2513480F7D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
     <sheet name="FlxTest10mm" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +24,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -375,6 +378,587 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2920603674540682E-2"/>
+                  <c:y val="-0.57792468649752116"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ExtTest10mm!$C$7:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-108.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-53.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ExtTest10mm!$C$15:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.284784415964447</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6607354242219894</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3254657241807237</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2208680746256029</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1169354947951735</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2307704310131626</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1875334409308596</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57276436046917911</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.37892854031665485</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DA6F-491E-B0B6-50DAB9D94DBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1167502896"/>
+        <c:axId val="1167503312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1167502896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1167503312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1167503312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1167502896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.64762025792611944"/>
+                  <c:y val="-9.2378640776699023E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6503408345745034E-2"/>
+                  <c:y val="-0.40305825242718446"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>FlxTest10mm!$C$7:$L$7</c:f>
@@ -687,6 +1271,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1203,7 +1827,564 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>692149</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>112183</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>374649</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>124883</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2120F2F-8116-4FA9-83EC-DF5046431D7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1543,28 +2724,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.1171875" style="5"/>
+    <col min="2" max="2" width="25.1171875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.29296875" customWidth="1"/>
+    <col min="5" max="5" width="8.703125" customWidth="1"/>
+    <col min="6" max="6" width="11.29296875" customWidth="1"/>
+    <col min="7" max="7" width="13.29296875" customWidth="1"/>
+    <col min="8" max="9" width="13.41015625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1572,7 +2753,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1581,7 +2762,7 @@
         <v>431.6</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1589,7 +2770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -1639,7 +2820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1671,7 +2852,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -1703,7 +2884,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -1744,7 +2925,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -1783,7 +2964,7 @@
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -1822,7 +3003,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -1830,7 +3011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
         <v>10</v>
@@ -1881,7 +3062,7 @@
         <v>366.05</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -1914,13 +3095,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
@@ -1988,6 +3169,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1995,28 +3177,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" activeCellId="1" sqref="C7:L7 C15:L15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.1171875" style="5"/>
+    <col min="2" max="2" width="19.703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.29296875" customWidth="1"/>
+    <col min="5" max="5" width="8.703125" customWidth="1"/>
+    <col min="6" max="6" width="11.29296875" customWidth="1"/>
+    <col min="7" max="7" width="13.29296875" customWidth="1"/>
+    <col min="8" max="9" width="13.41015625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -2024,7 +3206,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -2033,7 +3215,7 @@
         <v>344.45</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -2083,7 +3265,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -2118,7 +3300,7 @@
         <v>1.2350000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -2153,7 +3335,7 @@
         <v>-81</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -2196,7 +3378,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -2237,7 +3419,7 @@
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -2278,7 +3460,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -2301,7 +3483,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
         <v>10</v>
@@ -2352,7 +3534,7 @@
         <v>366.43</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -2388,13 +3570,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Saved results for different pinned extensor lengths
Saved results for different pinned extensor lengths
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA71BA0A-9BA8-4B23-BA76-2513480F7D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF64C379-7190-42A8-B10C-D2295AB7346E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
@@ -89,7 +89,7 @@
     <t>tendon</t>
   </si>
   <si>
-    <t>Flexsor Test 10mm</t>
+    <t>Flexor Test 10mm</t>
   </si>
 </sst>
 </file>
@@ -3177,9 +3177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>

</xml_diff>

<commit_message>
Created better plots. Saved figures.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF64C379-7190-42A8-B10C-D2295AB7346E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6FDC36-DA6D-4BBC-9FBF-E49119CF556F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-22500" yWindow="1230" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
@@ -436,6 +436,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.59266929725444728"/>
+                  <c:y val="-0.1581767821057766"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -477,14 +483,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="5"/>
+            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.2920603674540682E-2"/>
-                  <c:y val="-0.57792468649752116"/>
+                  <c:x val="-0.37717706774256526"/>
+                  <c:y val="-1.2529788864887464E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2724,28 +2730,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1171875" style="5"/>
-    <col min="2" max="2" width="25.1171875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.29296875" customWidth="1"/>
-    <col min="5" max="5" width="8.703125" customWidth="1"/>
-    <col min="6" max="6" width="11.29296875" customWidth="1"/>
-    <col min="7" max="7" width="13.29296875" customWidth="1"/>
-    <col min="8" max="9" width="13.41015625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -2753,7 +2759,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -2762,7 +2768,7 @@
         <v>431.6</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -2820,7 +2826,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -2852,7 +2858,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -2884,7 +2890,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -2925,7 +2931,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -2964,7 +2970,7 @@
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -3003,7 +3009,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -3011,7 +3017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
         <v>10</v>
@@ -3062,7 +3068,7 @@
         <v>366.05</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -3095,13 +3101,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
@@ -3177,26 +3183,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1171875" style="5"/>
-    <col min="2" max="2" width="19.703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.29296875" customWidth="1"/>
-    <col min="5" max="5" width="8.703125" customWidth="1"/>
-    <col min="6" max="6" width="11.29296875" customWidth="1"/>
-    <col min="7" max="7" width="13.29296875" customWidth="1"/>
-    <col min="8" max="9" width="13.41015625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -3204,7 +3210,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -3213,7 +3219,7 @@
         <v>344.45</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -3263,7 +3269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -3298,7 +3304,7 @@
         <v>1.2350000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>-81</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -3376,7 +3382,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -3417,7 +3423,7 @@
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -3458,7 +3464,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -3481,7 +3487,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
         <v>10</v>
@@ -3532,7 +3538,7 @@
         <v>366.43</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -3568,13 +3574,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Created more figures. Broke leg.
Created more figures for the report. Leg broke during testing of ExtTest2_2.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6FDC36-DA6D-4BBC-9FBF-E49119CF556F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73DA64F-EEAE-463A-B8EE-E0FFDA217830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22500" yWindow="1230" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-22995" yWindow="1320" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
     <sheet name="FlxTest10mm" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>Test #</t>
   </si>
@@ -90,6 +88,18 @@
   </si>
   <si>
     <t>Flexor Test 10mm</t>
+  </si>
+  <si>
+    <t>Vas_Pam insertion wrt arbitrary knee loc</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -2728,10 +2738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,6 +3179,60 @@
       </c>
       <c r="Q15">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>2.163E-2</v>
+      </c>
+      <c r="K23">
+        <v>-7.1639999999999995E-2</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>3.6389999999999999E-2</v>
+      </c>
+      <c r="K27">
+        <v>-6.3130000000000006E-2</v>
+      </c>
+      <c r="L27">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More figures, more robust code.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73DA64F-EEAE-463A-B8EE-E0FFDA217830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3C8D21-BD2A-4ECF-9B65-F21E2CDF47BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22995" yWindow="1320" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
@@ -2741,7 +2741,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="D33" sqref="D33:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on plots for bionic knee
10mm flexor and extensor. Making adjustments to plots and routing path for extensor. Hard to get everything to match.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3C8D21-BD2A-4ECF-9B65-F21E2CDF47BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F269656-E0D2-49C9-92A8-1AF48ED2C479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-28260" yWindow="1635" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
     <sheet name="FlxTest10mm" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Test #</t>
   </si>
@@ -90,9 +91,6 @@
     <t>Flexor Test 10mm</t>
   </si>
   <si>
-    <t>Vas_Pam insertion wrt arbitrary knee loc</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -100,6 +98,18 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>Vas_Pam insertion wrt proximal ring</t>
+  </si>
+  <si>
+    <t>Tendon Length</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -275,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -296,6 +306,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1075,6 +1088,8 @@
         <c:axId val="1052896735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="20"/>
+          <c:min val="-120"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1137,6 +1152,8 @@
         <c:axId val="1052895903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0"/>
+          <c:min val="-16"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2738,10 +2755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2777,6 +2794,12 @@
         <f>C2-C2*0.17</f>
         <v>431.6</v>
       </c>
+      <c r="D3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>440</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -2784,6 +2807,12 @@
       </c>
       <c r="C4">
         <v>30</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3184,55 +3213,28 @@
     </row>
     <row r="21" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22" t="s">
         <v>19</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>20</v>
-      </c>
-      <c r="L22" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="23" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J23">
-        <v>2.163E-2</v>
+        <v>2.053E-2</v>
       </c>
       <c r="K23">
-        <v>-7.1639999999999995E-2</v>
+        <v>-7.5569999999999998E-2</v>
       </c>
       <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J26" t="s">
-        <v>19</v>
-      </c>
-      <c r="K26" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J27">
-        <v>3.6389999999999999E-2</v>
-      </c>
-      <c r="K27">
-        <v>-6.3130000000000006E-2</v>
-      </c>
-      <c r="L27">
         <v>0</v>
       </c>
     </row>
@@ -3247,7 +3249,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:L13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3281,6 +3285,23 @@
       <c r="C3">
         <f>C2-C2*0.17</f>
         <v>344.45</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working on minimizing function
Minimizing function to reduce guess and check for curve fit
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F269656-E0D2-49C9-92A8-1AF48ED2C479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B153C1-11A8-47CE-AFA8-AB71D8A27CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28260" yWindow="1635" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-23805" yWindow="2940" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
     <sheet name="FlxTest10mm" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -903,8 +902,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.64762025792611944"/>
-                  <c:y val="-9.2378640776699023E-2"/>
+                  <c:x val="-0.48357939632545932"/>
+                  <c:y val="-0.10012284922717994"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -954,8 +953,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.6503408345745034E-2"/>
-                  <c:y val="-0.40305825242718446"/>
+                  <c:x val="-0.11580161854768153"/>
+                  <c:y val="0.13777048702245553"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -3249,8 +3248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:L13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Re-measured resting length and max contracted length
Also deleted autosave files
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE30732-EF84-4B06-906C-9BC7E902CC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6199F936-6F5B-400A-8124-6106A68DA6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17820" yWindow="915" windowWidth="13455" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-25740" yWindow="1200" windowWidth="13455" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished Bio Knee 10mm Flexor
FIgures and code is complete for the 10mm Flexor BPA used in the biomimetic knee.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6199F936-6F5B-400A-8124-6106A68DA6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6D175D-2A16-442E-A34E-9C2D639096A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25740" yWindow="1200" windowWidth="13455" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="21624" windowHeight="11244" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
     <sheet name="FlxTest10mm" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Test #</t>
   </si>
@@ -106,9 +109,6 @@
   </si>
   <si>
     <t>Tendon Length</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
@@ -284,12 +284,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -301,10 +299,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2756,116 +2750,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="25.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="9" width="13.44140625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2">
         <v>520</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C3">
         <f>C2-C2*0.17</f>
         <v>431.6</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E3">
         <v>440</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C4">
         <v>30</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E4">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <v>1</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>2</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>3</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <v>4</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="10">
         <v>5</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="10">
         <v>6</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="10">
         <v>7</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="10">
         <v>8</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="10">
         <v>9</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="10">
         <v>10</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="10">
         <v>11</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="10">
         <v>12</v>
       </c>
-      <c r="O5" s="12">
+      <c r="O5" s="10">
         <v>13</v>
       </c>
-      <c r="P5" s="12">
+      <c r="P5" s="10">
         <v>14</v>
       </c>
-      <c r="Q5" s="12">
+      <c r="Q5" s="10">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C6">
@@ -2896,8 +2890,8 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C7">
@@ -2928,225 +2922,207 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>33.6</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>36.700000000000003</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>36.1</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>39</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>34</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>38.5</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>36.4</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="1">
         <v>33.299999999999997</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="1">
         <v>34.6</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9">
         <v>30.5</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9">
         <v>30</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9">
         <v>34</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9">
         <v>42.5</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9">
         <v>40</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9">
         <v>41.5</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9">
         <v>38</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9">
         <v>38</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9">
         <v>35</v>
       </c>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C10">
         <v>518</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10">
         <v>520</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10">
         <v>510</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10">
         <v>495</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10">
         <v>485</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10">
         <v>475</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10">
         <v>460</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10">
         <v>450</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10">
         <v>450</v>
       </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12">
         <v>366.05</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12">
         <v>366.05</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12">
         <v>366.05</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12">
         <v>366.05</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12">
         <v>366.05</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12">
         <v>366.05</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12">
         <v>366.05</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12">
         <v>366.05</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12">
         <v>366.05</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12">
         <v>366.05</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12">
         <v>366.05</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12">
         <v>366.05</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12">
         <v>366.05</v>
       </c>
-      <c r="P12" s="16">
+      <c r="P12">
         <v>366.05</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12">
         <v>366.05</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13">
         <v>38</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13">
         <v>35</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13">
         <v>40</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13">
         <v>40</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13">
         <v>45</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13">
         <v>45</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13">
         <v>40</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13">
         <v>40</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C15">
@@ -3210,12 +3186,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J22" t="s">
         <v>18</v>
       </c>
@@ -3226,7 +3202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J23">
         <v>2.053E-2</v>
       </c>
@@ -3248,113 +3224,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="9" width="13.44140625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2">
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C3">
         <f>C2-C2*0.17</f>
         <v>344.45</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E3">
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>3</v>
+      </c>
+      <c r="F5" s="10">
+        <v>4</v>
+      </c>
+      <c r="G5" s="10">
+        <v>5</v>
+      </c>
+      <c r="H5" s="10">
+        <v>6</v>
+      </c>
+      <c r="I5" s="10">
+        <v>7</v>
+      </c>
+      <c r="J5" s="10">
+        <v>8</v>
+      </c>
+      <c r="K5" s="10">
+        <v>9</v>
+      </c>
+      <c r="L5" s="10">
+        <v>10</v>
+      </c>
+      <c r="M5" s="10">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>24</v>
+      <c r="N5" s="10">
+        <v>12</v>
+      </c>
+      <c r="O5" s="10">
+        <v>13</v>
+      </c>
+      <c r="P5" s="10">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="12">
-        <v>1</v>
-      </c>
-      <c r="D5" s="12">
-        <v>2</v>
-      </c>
-      <c r="E5" s="12">
-        <v>3</v>
-      </c>
-      <c r="F5" s="12">
-        <v>4</v>
-      </c>
-      <c r="G5" s="12">
-        <v>5</v>
-      </c>
-      <c r="H5" s="12">
-        <v>6</v>
-      </c>
-      <c r="I5" s="12">
-        <v>7</v>
-      </c>
-      <c r="J5" s="12">
-        <v>8</v>
-      </c>
-      <c r="K5" s="12">
-        <v>9</v>
-      </c>
-      <c r="L5" s="12">
-        <v>10</v>
-      </c>
-      <c r="M5" s="12">
-        <v>11</v>
-      </c>
-      <c r="N5" s="12">
-        <v>12</v>
-      </c>
-      <c r="O5" s="12">
-        <v>13</v>
-      </c>
-      <c r="P5" s="12">
-        <v>14</v>
-      </c>
-      <c r="Q5" s="12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C6">
@@ -3388,8 +3361,8 @@
         <v>1.2350000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C7">
@@ -3423,249 +3396,239 @@
         <v>-81</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>24</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>20</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>25.5</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>26.7</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>26.7</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>32.700000000000003</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="1">
         <v>29.75</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="1">
         <v>28.15</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="1">
         <v>37.9</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9">
         <v>23</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9">
         <v>23</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9">
         <v>21</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9">
         <v>23</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9">
         <v>28</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9">
         <v>28</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9">
         <v>29.5</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9">
         <v>34</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9">
         <v>34</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9">
         <v>41</v>
       </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C10">
         <v>397</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10">
         <v>390</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10">
         <v>387</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10">
         <v>380</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10">
         <v>375</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10">
         <v>371</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10">
         <v>367</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10">
         <v>365</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10">
         <v>365</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10">
         <v>357</v>
       </c>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12">
         <v>366.43</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12">
         <v>366.43</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12">
         <v>366.43</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12">
         <v>366.43</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12">
         <v>366.43</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12">
         <v>366.43</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12">
         <v>366.43</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12">
         <v>366.43</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12">
         <v>366.43</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12">
         <v>366.43</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12">
         <v>366.43</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12">
         <v>366.43</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12">
         <v>366.43</v>
       </c>
-      <c r="P12" s="16">
+      <c r="P12">
         <v>366.43</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12">
         <v>366.43</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13">
         <v>38</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13">
         <v>42</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13">
         <v>42</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13">
         <v>40</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13">
         <v>35</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13">
         <v>39</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13">
         <v>35</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13">
         <v>35</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13">
         <v>33</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C15">

</xml_diff>

<commit_message>
Modified ExtPin10mm plot scripts
Need to analyze and optimize data. Plotting scripts are good and standardized now.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6D175D-2A16-442E-A34E-9C2D639096A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CD882D-FB14-428D-AF2C-3161AEC0EBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="21624" windowHeight="11244" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="32925" yWindow="1965" windowWidth="21630" windowHeight="11250" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
@@ -2750,7 +2750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -3224,8 +3224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Now i just need a slice or something
find out how to make isolines
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782F277F-5E8B-45B6-B1ED-64BB3D81A09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE38220-AA7B-414A-A92B-1806E4BF0864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1158" yWindow="0" windowWidth="15672" windowHeight="12318" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
@@ -2921,28 +2921,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.15625" style="3"/>
-    <col min="2" max="2" width="25.15625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.26171875" customWidth="1"/>
-    <col min="5" max="5" width="8.68359375" customWidth="1"/>
-    <col min="6" max="6" width="11.26171875" customWidth="1"/>
-    <col min="7" max="7" width="13.26171875" customWidth="1"/>
-    <col min="8" max="9" width="13.41796875" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="25.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="9" width="13.44140625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>34.6</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
@@ -3161,7 +3161,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -3194,7 +3194,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -3253,7 +3253,7 @@
         <v>366.05</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -3286,13 +3286,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>25</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>0.29049999999999998</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>0.29330000000000001</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>0.2838</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>0.25900000000000001</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>2.9512999999999998</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>0.27129999999999999</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>2.8912</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>0.26690000000000003</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>2.0773000000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>0.28410000000000002</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>1.1246</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>0.28620000000000001</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>0.5464</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>0.29649999999999999</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>0.36180000000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30"/>
     </row>
   </sheetData>
@@ -3472,28 +3472,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9:L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.15625" style="3"/>
-    <col min="2" max="2" width="19.68359375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.26171875" customWidth="1"/>
-    <col min="5" max="5" width="8.68359375" customWidth="1"/>
-    <col min="6" max="6" width="11.26171875" customWidth="1"/>
-    <col min="7" max="7" width="13.26171875" customWidth="1"/>
-    <col min="8" max="9" width="13.41796875" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="9" width="13.44140625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>1.2350000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>-81</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>37.9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
@@ -3718,7 +3718,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -3759,7 +3759,7 @@
       <c r="P10"/>
       <c r="Q10"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -3782,7 +3782,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -3833,7 +3833,7 @@
         <v>366.43</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -3869,13 +3869,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Tried to refresh robot knee ICR to correct values. Now the graphs don't plot correct.
Check location matrix. Check p3 and p4 first, then check other wrapping points, then check knee ICr location.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FD8E68-EB48-4AD3-9F7D-3B725354300E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210B0E91-B4F8-4837-A784-1265E6471BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Test #</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Moment arm, actual (m)</t>
+  </si>
+  <si>
+    <t>kmax</t>
+  </si>
+  <si>
+    <t>avg. pres.</t>
+  </si>
+  <si>
+    <t>Pressure</t>
   </si>
 </sst>
 </file>
@@ -2623,9 +2632,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2663,7 +2672,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2769,7 +2778,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2911,7 +2920,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2919,30 +2928,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="25.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="25.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="9" width="13.44140625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -2950,7 +2959,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -2965,7 +2974,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
@@ -2979,7 +2988,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -3029,7 +3038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -3061,7 +3070,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -3093,7 +3102,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -3128,7 +3137,7 @@
         <v>34.6</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
@@ -3161,7 +3170,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -3194,7 +3203,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -3202,7 +3211,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -3253,7 +3262,7 @@
         <v>366.05</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -3286,13 +3295,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
@@ -3357,7 +3366,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>601.48289999999997</v>
+      </c>
+      <c r="D17">
+        <v>600.72787878787904</v>
+      </c>
+      <c r="E17">
+        <v>585.37148582600196</v>
+      </c>
+      <c r="F17">
+        <v>597.24558162267795</v>
+      </c>
+      <c r="G17">
+        <v>595.76131964809395</v>
+      </c>
+      <c r="H17">
+        <v>597.24558162267795</v>
+      </c>
+      <c r="I17">
+        <v>597.24558162267795</v>
+      </c>
+      <c r="J17">
+        <v>596.503450635386</v>
+      </c>
+      <c r="K17">
+        <v>595.76131964809395</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>25</v>
       </c>
@@ -3365,7 +3406,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>0.29049999999999998</v>
       </c>
@@ -3376,7 +3417,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>0.29330000000000001</v>
       </c>
@@ -3392,8 +3433,15 @@
       <c r="L22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="R22" t="s">
+        <v>26</v>
+      </c>
+      <c r="S22">
+        <f>1-440/520</f>
+        <v>0.15384615384615385</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>0.2838</v>
       </c>
@@ -3409,8 +3457,15 @@
       <c r="L23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="R23" t="s">
+        <v>27</v>
+      </c>
+      <c r="S23">
+        <f>SUM(C17:K17)/9</f>
+        <v>596.37167771260988</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>0.25900000000000001</v>
       </c>
@@ -3418,7 +3473,7 @@
         <v>2.9512999999999998</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>0.27129999999999999</v>
       </c>
@@ -3426,7 +3481,7 @@
         <v>2.8912</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>0.26690000000000003</v>
       </c>
@@ -3434,7 +3489,7 @@
         <v>2.0773000000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>0.28410000000000002</v>
       </c>
@@ -3442,7 +3497,7 @@
         <v>1.1246</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>0.28620000000000001</v>
       </c>
@@ -3450,7 +3505,7 @@
         <v>0.5464</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>0.29649999999999999</v>
       </c>
@@ -3458,7 +3513,7 @@
         <v>0.36180000000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B30"/>
     </row>
   </sheetData>
@@ -3472,28 +3527,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="9" width="13.44140625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -3501,7 +3556,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
@@ -3516,7 +3571,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
@@ -3524,7 +3579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -3574,7 +3629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -3609,7 +3664,7 @@
         <v>1.2350000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
@@ -3644,7 +3699,7 @@
         <v>-81</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -3682,7 +3737,7 @@
         <v>37.9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
@@ -3718,7 +3773,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -3759,7 +3814,7 @@
       <c r="P10"/>
       <c r="Q10"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
@@ -3782,7 +3837,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -3833,7 +3888,7 @@
         <v>366.43</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>11</v>
@@ -3869,13 +3924,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>

</xml_diff>